<commit_message>
tried to fit the curves to tests
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kutla\Documents\GitHub\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F695EF0-B691-4318-BD09-CE6F1D21BBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE055C59-9A99-4323-9ED4-E18770A997CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="21600" windowHeight="12735" xr2:uid="{F7DBB6B4-45F2-4430-91CB-563ABD69A36A}"/>
+    <workbookView xWindow="330" yWindow="345" windowWidth="21600" windowHeight="12735" xr2:uid="{F7DBB6B4-45F2-4430-91CB-563ABD69A36A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.42941639999999998</v>
+        <v>0.57255529999999999</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.7974</v>
+        <v>0.95</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -491,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>5.4400000000000001E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>1.4559999999999999E-4</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>3.0620000000000001E-2</v>
+        <v>3.7749999999999999E-2</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>2.8892000000000002E-3</v>
+        <v>6.8110000000000002E-4</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>5.0000000000000001E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -579,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1.272E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>1.1107999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -612,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>1.7279999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>2.9480000000000001E-3</v>
+        <v>4.3499999999999997E-3</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>2.9480000000000001E-3</v>
+        <v>1.65E-3</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>

</xml_diff>